<commit_message>
add custom cleavage Aug-12-2025
</commit_message>
<xml_diff>
--- a/pytheas_data/pytheas_global_parameters.xlsx
+++ b/pytheas_data/pytheas_global_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrwill/prog/Pytheas_Folder/Pytheas_Qt_root/Pytheas_Qt/pytheas_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAF55BD-698C-F542-BEB5-5FA535C38D71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6937480D-19B2-284B-BA55-426B5884437E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8860" yWindow="1540" windowWidth="32900" windowHeight="21200" xr2:uid="{5EC5A63B-1C8A-8A4B-9184-3058BFCD8B26}"/>
+    <workbookView xWindow="13820" yWindow="1160" windowWidth="32900" windowHeight="21200" xr2:uid="{5EC5A63B-1C8A-8A4B-9184-3058BFCD8B26}"/>
   </bookViews>
   <sheets>
     <sheet name="pytheas_button_parameters" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="335">
   <si>
     <t>missed_cleavages</t>
   </si>
@@ -1033,6 +1033,12 @@
   </si>
   <si>
     <t>optional input</t>
+  </si>
+  <si>
+    <t>Custom Cleavage definitions</t>
+  </si>
+  <si>
+    <t>custom_cleavage_file</t>
   </si>
 </sst>
 </file>
@@ -1401,8 +1407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA26392-E153-8845-A8FA-3CAC8BC5DFBF}">
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="118" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" zoomScale="118" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1891,10 +1897,10 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>256</v>
+        <v>333</v>
       </c>
       <c r="B14" t="s">
-        <v>257</v>
+        <v>334</v>
       </c>
       <c r="C14" t="s">
         <v>214</v>
@@ -1924,7 +1930,7 @@
         <v>119</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>202</v>
+        <v>123</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>332</v>

</xml_diff>

<commit_message>
command line arguments implemented, patches to digest plot, global parameter patch, option menu reorg
</commit_message>
<xml_diff>
--- a/pytheas_data/pytheas_global_parameters.xlsx
+++ b/pytheas_data/pytheas_global_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrwill/prog/Pytheas_Folder/Pytheas_Qt_root/Pytheas_Qt/pytheas_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E93CBD-E334-6C48-B3C4-0E395C206889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BED0F5-859B-D148-88DE-7D5ECE8FDBF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14260" yWindow="6160" windowWidth="32900" windowHeight="21200" xr2:uid="{5EC5A63B-1C8A-8A4B-9184-3058BFCD8B26}"/>
+    <workbookView xWindow="800" yWindow="760" windowWidth="28600" windowHeight="18360" xr2:uid="{5EC5A63B-1C8A-8A4B-9184-3058BFCD8B26}"/>
   </bookViews>
   <sheets>
     <sheet name="pytheas_button_parameters" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="958" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="962" uniqueCount="357">
   <si>
     <t>missed_cleavages</t>
   </si>
@@ -636,9 +636,6 @@
     <t>Output filenames (Work Directory)</t>
   </si>
   <si>
-    <t>pytheas_parameters.xlsx</t>
-  </si>
-  <si>
     <t>used in digest</t>
   </si>
   <si>
@@ -738,9 +735,6 @@
     <t>RNA Modifications:</t>
   </si>
   <si>
-    <t>Modifications and Labeling</t>
-  </si>
-  <si>
     <t>output_files</t>
   </si>
   <si>
@@ -1038,9 +1032,6 @@
     <t>custom_cleavage_file</t>
   </si>
   <si>
-    <t>Standard File Nmaes</t>
-  </si>
-  <si>
     <t>natural,training_set,yeast_tRNA_set,Psa_trna_set,human_rRNA_set</t>
   </si>
   <si>
@@ -1099,6 +1090,21 @@
   </si>
   <si>
     <t>Base Labels in Seq Map</t>
+  </si>
+  <si>
+    <t>pytheas_recent_parameters.xlsx</t>
+  </si>
+  <si>
+    <t>hide</t>
+  </si>
+  <si>
+    <t>Mods and Labeling</t>
+  </si>
+  <si>
+    <t>Output options</t>
+  </si>
+  <si>
+    <t>Plot options</t>
   </si>
 </sst>
 </file>
@@ -1465,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA26392-E153-8845-A8FA-3CAC8BC5DFBF}">
-  <dimension ref="A1:M104"/>
+  <dimension ref="A1:N104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="118" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="118" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E78" sqref="E78:E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1482,10 +1488,10 @@
     <col min="7" max="7" width="9.6640625" customWidth="1"/>
     <col min="8" max="8" width="37" style="1" customWidth="1"/>
     <col min="9" max="11" width="28.1640625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="2" customWidth="1"/>
+    <col min="12" max="13" width="10.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -1522,11 +1528,14 @@
       <c r="L1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="N1" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>135</v>
       </c>
@@ -1534,7 +1543,7 @@
         <v>136</v>
       </c>
       <c r="C2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D2" t="s">
         <v>94</v>
@@ -1555,7 +1564,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>116</v>
       </c>
@@ -1563,7 +1572,7 @@
         <v>119</v>
       </c>
       <c r="C3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D3" t="s">
         <v>94</v>
@@ -1581,13 +1590,13 @@
         <v>71</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L3" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -1595,7 +1604,7 @@
         <v>120</v>
       </c>
       <c r="C4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
         <v>94</v>
@@ -1613,13 +1622,13 @@
         <v>71</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -1627,7 +1636,7 @@
         <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D5" t="s">
         <v>94</v>
@@ -1645,13 +1654,13 @@
         <v>71</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -1659,7 +1668,7 @@
         <v>139</v>
       </c>
       <c r="C6" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D6" t="s">
         <v>76</v>
@@ -1680,7 +1689,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>48</v>
       </c>
@@ -1688,7 +1697,7 @@
         <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D7" t="s">
         <v>76</v>
@@ -1697,7 +1706,7 @@
         <v>76</v>
       </c>
       <c r="F7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G7" t="s">
         <v>70</v>
@@ -1706,7 +1715,7 @@
         <v>71</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>145</v>
@@ -1717,19 +1726,19 @@
       <c r="L7" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D8" t="s">
         <v>76</v>
@@ -1738,7 +1747,7 @@
         <v>76</v>
       </c>
       <c r="F8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G8" t="s">
         <v>70</v>
@@ -1747,10 +1756,10 @@
         <v>71</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>119</v>
@@ -1758,11 +1767,11 @@
       <c r="L8" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>53</v>
       </c>
@@ -1770,7 +1779,7 @@
         <v>129</v>
       </c>
       <c r="C9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D9" t="s">
         <v>76</v>
@@ -1779,7 +1788,7 @@
         <v>76</v>
       </c>
       <c r="F9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G9" t="s">
         <v>70</v>
@@ -1788,7 +1797,7 @@
         <v>131</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>146</v>
@@ -1797,13 +1806,13 @@
         <v>121</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="M9" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N9" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>141</v>
       </c>
@@ -1811,7 +1820,7 @@
         <v>142</v>
       </c>
       <c r="C10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D10" t="s">
         <v>77</v>
@@ -1832,7 +1841,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -1840,7 +1849,7 @@
         <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D11" t="s">
         <v>77</v>
@@ -1849,7 +1858,7 @@
         <v>77</v>
       </c>
       <c r="F11" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G11" t="s">
         <v>70</v>
@@ -1858,7 +1867,7 @@
         <v>71</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J11" s="2" t="s">
         <v>147</v>
@@ -1869,11 +1878,11 @@
       <c r="L11" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -1881,7 +1890,7 @@
         <v>130</v>
       </c>
       <c r="C12" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D12" t="s">
         <v>77</v>
@@ -1890,7 +1899,7 @@
         <v>77</v>
       </c>
       <c r="F12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G12" t="s">
         <v>70</v>
@@ -1899,7 +1908,7 @@
         <v>71</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>146</v>
@@ -1908,21 +1917,21 @@
         <v>121</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="M12" s="2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N12" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B13" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="C13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D13" t="s">
         <v>77</v>
@@ -1931,19 +1940,19 @@
         <v>77</v>
       </c>
       <c r="F13" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G13" t="s">
         <v>70</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>119</v>
@@ -1951,11 +1960,11 @@
       <c r="L13" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M13" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N13" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -1963,7 +1972,7 @@
         <v>90</v>
       </c>
       <c r="C14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D14" t="s">
         <v>163</v>
@@ -1984,15 +1993,15 @@
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B15" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="C15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D15" t="s">
         <v>163</v>
@@ -2001,7 +2010,7 @@
         <v>158</v>
       </c>
       <c r="F15" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="G15" t="s">
         <v>58</v>
@@ -2010,10 +2019,10 @@
         <v>62</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -2021,7 +2030,7 @@
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D16" t="s">
         <v>163</v>
@@ -2042,7 +2051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -2050,7 +2059,7 @@
         <v>17</v>
       </c>
       <c r="C17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D17" t="s">
         <v>163</v>
@@ -2071,7 +2080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -2079,7 +2088,7 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D18" t="s">
         <v>163</v>
@@ -2100,7 +2109,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>7</v>
       </c>
@@ -2108,7 +2117,7 @@
         <v>154</v>
       </c>
       <c r="C19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D19" t="s">
         <v>163</v>
@@ -2129,7 +2138,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -2137,7 +2146,7 @@
         <v>155</v>
       </c>
       <c r="C20" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D20" t="s">
         <v>163</v>
@@ -2158,7 +2167,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -2166,7 +2175,7 @@
         <v>152</v>
       </c>
       <c r="C21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D21" t="s">
         <v>163</v>
@@ -2187,7 +2196,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -2195,7 +2204,7 @@
         <v>153</v>
       </c>
       <c r="C22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D22" t="s">
         <v>163</v>
@@ -2216,7 +2225,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -2224,7 +2233,7 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D23" t="s">
         <v>163</v>
@@ -2245,7 +2254,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -2253,7 +2262,7 @@
         <v>96</v>
       </c>
       <c r="C24" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D24" t="s">
         <v>163</v>
@@ -2274,24 +2283,24 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B25" t="s">
         <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D25" t="s">
         <v>163</v>
       </c>
       <c r="E25" t="s">
-        <v>234</v>
+        <v>354</v>
       </c>
       <c r="F25" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G25" t="s">
         <v>56</v>
@@ -2303,7 +2312,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>171</v>
       </c>
@@ -2311,13 +2320,13 @@
         <v>172</v>
       </c>
       <c r="C26" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D26" t="s">
         <v>163</v>
       </c>
       <c r="E26" t="s">
-        <v>234</v>
+        <v>354</v>
       </c>
       <c r="F26" t="s">
         <v>174</v>
@@ -2329,27 +2338,27 @@
         <v>173</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B27" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C27" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D27" t="s">
         <v>163</v>
       </c>
       <c r="E27" t="s">
-        <v>234</v>
+        <v>354</v>
       </c>
       <c r="F27" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="G27" t="s">
         <v>56</v>
@@ -2361,7 +2370,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -2369,13 +2378,13 @@
         <v>29</v>
       </c>
       <c r="C28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D28" t="s">
         <v>163</v>
       </c>
       <c r="E28" t="s">
-        <v>234</v>
+        <v>354</v>
       </c>
       <c r="F28" t="s">
         <v>29</v>
@@ -2390,24 +2399,24 @@
         <v>107</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B29" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C29" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D29" t="s">
         <v>163</v>
       </c>
       <c r="E29" t="s">
-        <v>234</v>
+        <v>354</v>
       </c>
       <c r="F29" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="G29" t="s">
         <v>56</v>
@@ -2419,7 +2428,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2427,7 +2436,7 @@
         <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D30" t="s">
         <v>163</v>
@@ -2448,7 +2457,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -2456,7 +2465,7 @@
         <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D31" t="s">
         <v>163</v>
@@ -2479,8 +2488,9 @@
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M31" s="3"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2488,7 +2498,7 @@
         <v>22</v>
       </c>
       <c r="C32" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D32" t="s">
         <v>163</v>
@@ -2509,7 +2519,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>23</v>
       </c>
@@ -2517,7 +2527,7 @@
         <v>23</v>
       </c>
       <c r="C33" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D33" t="s">
         <v>163</v>
@@ -2538,7 +2548,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>24</v>
       </c>
@@ -2546,7 +2556,7 @@
         <v>24</v>
       </c>
       <c r="C34" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D34" t="s">
         <v>163</v>
@@ -2567,7 +2577,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>25</v>
       </c>
@@ -2575,7 +2585,7 @@
         <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D35" t="s">
         <v>163</v>
@@ -2596,7 +2606,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>26</v>
       </c>
@@ -2604,7 +2614,7 @@
         <v>26</v>
       </c>
       <c r="C36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D36" t="s">
         <v>163</v>
@@ -2619,21 +2629,21 @@
         <v>58</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B37" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C37" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D37" t="s">
         <v>163</v>
@@ -2642,7 +2652,7 @@
         <v>159</v>
       </c>
       <c r="F37" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G37" t="s">
         <v>56</v>
@@ -2651,27 +2661,27 @@
         <v>30</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="B38" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D38" t="s">
         <v>163</v>
       </c>
       <c r="E38" t="s">
-        <v>159</v>
+        <v>355</v>
       </c>
       <c r="F38" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="G38" t="s">
         <v>56</v>
@@ -2683,24 +2693,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="B39" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C39" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D39" t="s">
         <v>163</v>
       </c>
       <c r="E39" t="s">
-        <v>159</v>
+        <v>355</v>
       </c>
       <c r="F39" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="G39" t="s">
         <v>56</v>
@@ -2712,24 +2722,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="B40" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C40" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D40" t="s">
         <v>163</v>
       </c>
       <c r="E40" t="s">
-        <v>159</v>
+        <v>355</v>
       </c>
       <c r="F40" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="G40" t="s">
         <v>56</v>
@@ -2741,7 +2751,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>175</v>
       </c>
@@ -2749,7 +2759,7 @@
         <v>176</v>
       </c>
       <c r="C41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D41" t="s">
         <v>163</v>
@@ -2769,8 +2779,11 @@
       <c r="I41" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M41" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>179</v>
       </c>
@@ -2778,7 +2791,7 @@
         <v>180</v>
       </c>
       <c r="C42" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D42" t="s">
         <v>163</v>
@@ -2798,8 +2811,11 @@
       <c r="I42" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M42" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>181</v>
       </c>
@@ -2807,7 +2823,7 @@
         <v>182</v>
       </c>
       <c r="C43" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D43" t="s">
         <v>163</v>
@@ -2827,8 +2843,11 @@
       <c r="I43" s="2" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M43" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>82</v>
       </c>
@@ -2836,7 +2855,7 @@
         <v>83</v>
       </c>
       <c r="C44" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D44" t="s">
         <v>164</v>
@@ -2857,7 +2876,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>31</v>
       </c>
@@ -2865,7 +2884,7 @@
         <v>31</v>
       </c>
       <c r="C45" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D45" t="s">
         <v>164</v>
@@ -2888,8 +2907,9 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>32</v>
       </c>
@@ -2897,7 +2917,7 @@
         <v>32</v>
       </c>
       <c r="C46" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D46" t="s">
         <v>164</v>
@@ -2920,8 +2940,9 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M46" s="1"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>33</v>
       </c>
@@ -2929,7 +2950,7 @@
         <v>33</v>
       </c>
       <c r="C47" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D47" t="s">
         <v>164</v>
@@ -2952,8 +2973,9 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M47" s="1"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>34</v>
       </c>
@@ -2961,7 +2983,7 @@
         <v>34</v>
       </c>
       <c r="C48" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D48" t="s">
         <v>164</v>
@@ -2984,8 +3006,9 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M48" s="1"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -2993,7 +3016,7 @@
         <v>41</v>
       </c>
       <c r="C49" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D49" t="s">
         <v>164</v>
@@ -3014,7 +3037,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>40</v>
       </c>
@@ -3022,7 +3045,7 @@
         <v>40</v>
       </c>
       <c r="C50" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D50" t="s">
         <v>164</v>
@@ -3043,7 +3066,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>73</v>
       </c>
@@ -3051,7 +3074,7 @@
         <v>73</v>
       </c>
       <c r="C51" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D51" t="s">
         <v>164</v>
@@ -3072,7 +3095,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>84</v>
       </c>
@@ -3080,7 +3103,7 @@
         <v>85</v>
       </c>
       <c r="C52" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D52" t="s">
         <v>164</v>
@@ -3101,7 +3124,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>36</v>
       </c>
@@ -3109,7 +3132,7 @@
         <v>36</v>
       </c>
       <c r="C53" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D53" t="s">
         <v>164</v>
@@ -3132,8 +3155,9 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M53" s="1"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>185</v>
       </c>
@@ -3141,7 +3165,7 @@
         <v>185</v>
       </c>
       <c r="C54" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D54" t="s">
         <v>164</v>
@@ -3164,8 +3188,9 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M54" s="1"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>187</v>
       </c>
@@ -3173,7 +3198,7 @@
         <v>187</v>
       </c>
       <c r="C55" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D55" t="s">
         <v>164</v>
@@ -3196,8 +3221,9 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M55" s="1"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>37</v>
       </c>
@@ -3205,7 +3231,7 @@
         <v>37</v>
       </c>
       <c r="C56" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D56" t="s">
         <v>164</v>
@@ -3228,19 +3254,20 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
-      <c r="M56" t="s">
+      <c r="M56" s="1"/>
+      <c r="N56" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B57" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C57" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D57" t="s">
         <v>164</v>
@@ -3249,7 +3276,7 @@
         <v>161</v>
       </c>
       <c r="F57" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G57" t="s">
         <v>56</v>
@@ -3263,11 +3290,12 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
-      <c r="M57" t="s">
+      <c r="M57" s="1"/>
+      <c r="N57" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>87</v>
       </c>
@@ -3275,7 +3303,7 @@
         <v>86</v>
       </c>
       <c r="C58" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D58" t="s">
         <v>164</v>
@@ -3296,7 +3324,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -3304,7 +3332,7 @@
         <v>38</v>
       </c>
       <c r="C59" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D59" t="s">
         <v>164</v>
@@ -3327,8 +3355,9 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M59" s="1"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>39</v>
       </c>
@@ -3336,7 +3365,7 @@
         <v>39</v>
       </c>
       <c r="C60" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D60" t="s">
         <v>164</v>
@@ -3359,8 +3388,9 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M60" s="1"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>35</v>
       </c>
@@ -3368,7 +3398,7 @@
         <v>35</v>
       </c>
       <c r="C61" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D61" t="s">
         <v>164</v>
@@ -3391,8 +3421,9 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M61" s="1"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>193</v>
       </c>
@@ -3400,7 +3431,7 @@
         <v>193</v>
       </c>
       <c r="C62" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D62" t="s">
         <v>164</v>
@@ -3423,16 +3454,17 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M62" s="1"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B63" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C63" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D63" t="s">
         <v>164</v>
@@ -3441,7 +3473,7 @@
         <v>162</v>
       </c>
       <c r="F63" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G63" t="s">
         <v>57</v>
@@ -3455,16 +3487,17 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M63" s="1"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B64" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C64" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D64" t="s">
         <v>164</v>
@@ -3473,7 +3506,7 @@
         <v>162</v>
       </c>
       <c r="F64" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G64" t="s">
         <v>57</v>
@@ -3487,16 +3520,17 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M64" s="1"/>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B65" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C65" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D65" t="s">
         <v>164</v>
@@ -3505,7 +3539,7 @@
         <v>162</v>
       </c>
       <c r="F65" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="G65" t="s">
         <v>59</v>
@@ -3519,16 +3553,17 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M65" s="1"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
+        <v>227</v>
+      </c>
+      <c r="B66" t="s">
         <v>228</v>
       </c>
-      <c r="B66" t="s">
-        <v>229</v>
-      </c>
       <c r="C66" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D66" t="s">
         <v>164</v>
@@ -3537,30 +3572,31 @@
         <v>162</v>
       </c>
       <c r="F66" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G66" t="s">
         <v>56</v>
       </c>
       <c r="H66" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="I66" s="1" t="s">
         <v>230</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>231</v>
       </c>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M66" s="1"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B67" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C67" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D67" t="s">
         <v>164</v>
@@ -3569,7 +3605,7 @@
         <v>162</v>
       </c>
       <c r="F67" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G67" t="s">
         <v>56</v>
@@ -3583,16 +3619,17 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M67" s="1"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B68" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C68" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D68" t="s">
         <v>164</v>
@@ -3601,7 +3638,7 @@
         <v>162</v>
       </c>
       <c r="F68" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G68" t="s">
         <v>56</v>
@@ -3615,8 +3652,9 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M68" s="1"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>195</v>
       </c>
@@ -3624,7 +3662,7 @@
         <v>197</v>
       </c>
       <c r="C69" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D69" t="s">
         <v>164</v>
@@ -3645,24 +3683,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B70" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C70" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D70" t="s">
         <v>164</v>
       </c>
       <c r="E70" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F70" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G70" t="s">
         <v>56</v>
@@ -3674,24 +3712,24 @@
         <v>71</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B71" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C71" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D71" t="s">
         <v>164</v>
       </c>
       <c r="E71" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F71" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="G71" t="s">
         <v>57</v>
@@ -3703,24 +3741,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="B72" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C72" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D72" t="s">
         <v>164</v>
       </c>
       <c r="E72" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F72" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G72" t="s">
         <v>59</v>
@@ -3732,120 +3770,123 @@
         <v>7.4999999999999997E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B73" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C73" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D73" t="s">
         <v>164</v>
       </c>
       <c r="E73" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F73" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G73" t="s">
         <v>58</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M73" s="1"/>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B74" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="C74" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D74" t="s">
         <v>164</v>
       </c>
       <c r="E74" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F74" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G74" t="s">
         <v>58</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M74" s="1"/>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B75" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C75" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D75" t="s">
         <v>164</v>
       </c>
       <c r="E75" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F75" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G75" t="s">
         <v>58</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M75" s="1"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="B76" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C76" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D76" t="s">
         <v>164</v>
       </c>
       <c r="E76" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F76" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="G76" t="s">
         <v>56</v>
@@ -3859,25 +3900,26 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M76" s="1"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="B77" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C77" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D77" t="s">
         <v>164</v>
       </c>
       <c r="E77" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F77" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="G77" t="s">
         <v>56</v>
@@ -3891,25 +3933,26 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M77" s="1"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B78" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C78" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D78" t="s">
         <v>164</v>
       </c>
       <c r="E78" t="s">
-        <v>239</v>
+        <v>356</v>
       </c>
       <c r="F78" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G78" t="s">
         <v>56</v>
@@ -3921,7 +3964,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>191</v>
       </c>
@@ -3929,13 +3972,13 @@
         <v>191</v>
       </c>
       <c r="C79" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D79" t="s">
         <v>164</v>
       </c>
       <c r="E79" t="s">
-        <v>239</v>
+        <v>356</v>
       </c>
       <c r="F79" t="s">
         <v>192</v>
@@ -3952,25 +3995,26 @@
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M79" s="1"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B80" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C80" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D80" t="s">
         <v>164</v>
       </c>
       <c r="E80" t="s">
-        <v>239</v>
+        <v>356</v>
       </c>
       <c r="F80" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G80" t="s">
         <v>56</v>
@@ -3984,25 +4028,26 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M80" s="1"/>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B81" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C81" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D81" t="s">
         <v>164</v>
       </c>
       <c r="E81" t="s">
-        <v>239</v>
+        <v>356</v>
       </c>
       <c r="F81" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G81" t="s">
         <v>56</v>
@@ -4016,25 +4061,26 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
-    </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M81" s="1"/>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B82" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C82" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D82" t="s">
         <v>164</v>
       </c>
       <c r="E82" t="s">
-        <v>239</v>
+        <v>356</v>
       </c>
       <c r="F82" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G82" t="s">
         <v>56</v>
@@ -4048,57 +4094,59 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M82" s="1"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B83" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C83" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D83" t="s">
         <v>164</v>
       </c>
       <c r="E83" t="s">
-        <v>239</v>
+        <v>356</v>
       </c>
       <c r="F83" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G83" t="s">
         <v>58</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
-    </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M83" s="1"/>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
+        <v>248</v>
+      </c>
+      <c r="B84" t="s">
+        <v>249</v>
+      </c>
+      <c r="C84" t="s">
+        <v>211</v>
+      </c>
+      <c r="D84" t="s">
+        <v>248</v>
+      </c>
+      <c r="E84" t="s">
         <v>250</v>
       </c>
-      <c r="B84" t="s">
-        <v>251</v>
-      </c>
-      <c r="C84" t="s">
-        <v>212</v>
-      </c>
-      <c r="D84" t="s">
-        <v>250</v>
-      </c>
-      <c r="E84" t="s">
-        <v>252</v>
-      </c>
       <c r="F84" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G84" t="s">
         <v>56</v>
@@ -4112,57 +4160,59 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
       <c r="L84" s="1"/>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M84" s="1"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B85" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="C85" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D85" t="s">
+        <v>248</v>
+      </c>
+      <c r="E85" t="s">
         <v>250</v>
       </c>
-      <c r="E85" t="s">
-        <v>252</v>
-      </c>
       <c r="F85" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G85" t="s">
         <v>58</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M85" s="1"/>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
+        <v>258</v>
+      </c>
+      <c r="B86" t="s">
+        <v>259</v>
+      </c>
+      <c r="C86" t="s">
+        <v>214</v>
+      </c>
+      <c r="D86" t="s">
+        <v>248</v>
+      </c>
+      <c r="E86" t="s">
+        <v>250</v>
+      </c>
+      <c r="F86" t="s">
         <v>260</v>
-      </c>
-      <c r="B86" t="s">
-        <v>261</v>
-      </c>
-      <c r="C86" t="s">
-        <v>215</v>
-      </c>
-      <c r="D86" t="s">
-        <v>250</v>
-      </c>
-      <c r="E86" t="s">
-        <v>252</v>
-      </c>
-      <c r="F86" t="s">
-        <v>262</v>
       </c>
       <c r="G86" t="s">
         <v>57</v>
@@ -4171,30 +4221,31 @@
         <v>16</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M86" s="1"/>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="B87" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C87" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D87" t="s">
+        <v>248</v>
+      </c>
+      <c r="E87" t="s">
         <v>250</v>
       </c>
-      <c r="E87" t="s">
-        <v>252</v>
-      </c>
       <c r="F87" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G87" t="s">
         <v>57</v>
@@ -4208,25 +4259,26 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M87" s="1"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B88" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C88" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D88" t="s">
+        <v>248</v>
+      </c>
+      <c r="E88" t="s">
         <v>250</v>
       </c>
-      <c r="E88" t="s">
-        <v>252</v>
-      </c>
       <c r="F88" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="G88" t="s">
         <v>57</v>
@@ -4240,25 +4292,26 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M88" s="1"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="B89" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C89" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D89" t="s">
+        <v>248</v>
+      </c>
+      <c r="E89" t="s">
         <v>250</v>
       </c>
-      <c r="E89" t="s">
-        <v>252</v>
-      </c>
       <c r="F89" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G89" t="s">
         <v>56</v>
@@ -4272,25 +4325,26 @@
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M89" s="1"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="B90" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C90" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D90" t="s">
+        <v>248</v>
+      </c>
+      <c r="E90" t="s">
         <v>250</v>
       </c>
-      <c r="E90" t="s">
-        <v>252</v>
-      </c>
       <c r="F90" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="G90" t="s">
         <v>59</v>
@@ -4299,10 +4353,10 @@
         <v>0.2</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>126</v>
       </c>
@@ -4310,7 +4364,7 @@
         <v>128</v>
       </c>
       <c r="C91" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D91" t="s">
         <v>198</v>
@@ -4328,7 +4382,7 @@
         <v>127</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J91" s="2" t="s">
         <v>148</v>
@@ -4337,13 +4391,13 @@
         <v>121</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="M91" t="s">
+        <v>201</v>
+      </c>
+      <c r="N91" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>98</v>
       </c>
@@ -4351,7 +4405,7 @@
         <v>99</v>
       </c>
       <c r="C92" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D92" t="s">
         <v>198</v>
@@ -4369,7 +4423,7 @@
         <v>101</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J92" s="2" t="s">
         <v>151</v>
@@ -4378,13 +4432,13 @@
         <v>121</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="M92" t="s">
+        <v>201</v>
+      </c>
+      <c r="N92" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>109</v>
       </c>
@@ -4392,7 +4446,7 @@
         <v>115</v>
       </c>
       <c r="C93" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D93" t="s">
         <v>198</v>
@@ -4410,7 +4464,7 @@
         <v>110</v>
       </c>
       <c r="I93" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J93" s="2" t="s">
         <v>149</v>
@@ -4419,13 +4473,13 @@
         <v>121</v>
       </c>
       <c r="L93" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="M93" t="s">
+        <v>201</v>
+      </c>
+      <c r="N93" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>111</v>
       </c>
@@ -4433,7 +4487,7 @@
         <v>112</v>
       </c>
       <c r="C94" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D94" t="s">
         <v>198</v>
@@ -4451,7 +4505,7 @@
         <v>114</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J94" s="2" t="s">
         <v>150</v>
@@ -4460,13 +4514,13 @@
         <v>121</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="M94" t="s">
+        <v>201</v>
+      </c>
+      <c r="N94" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>166</v>
       </c>
@@ -4474,7 +4528,7 @@
         <v>167</v>
       </c>
       <c r="C95" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D95" t="s">
         <v>198</v>
@@ -4492,7 +4546,7 @@
         <v>169</v>
       </c>
       <c r="I95" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J95" s="2" t="s">
         <v>165</v>
@@ -4501,62 +4555,62 @@
         <v>121</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="M95" t="s">
+        <v>201</v>
+      </c>
+      <c r="N95" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B96" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C96" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D96" t="s">
-        <v>334</v>
+        <v>198</v>
       </c>
       <c r="E96" t="s">
         <v>157</v>
       </c>
       <c r="F96" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="G96" t="s">
         <v>70</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="I96" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J96" s="2" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K96" s="2" t="s">
         <v>121</v>
       </c>
       <c r="L96" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="M96" s="2" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+      <c r="N96" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>222</v>
+      </c>
+      <c r="B97" t="s">
         <v>223</v>
       </c>
-      <c r="B97" t="s">
-        <v>224</v>
-      </c>
       <c r="C97" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D97" t="s">
         <v>198</v>
@@ -4565,45 +4619,45 @@
         <v>157</v>
       </c>
       <c r="F97" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="G97" t="s">
         <v>70</v>
       </c>
       <c r="H97" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="I97" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="J97" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="I97" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="J97" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="K97" s="2" t="s">
         <v>121</v>
       </c>
       <c r="L97" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="M97" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="N97" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
+        <v>209</v>
+      </c>
+      <c r="B98" t="s">
         <v>210</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" t="s">
         <v>211</v>
-      </c>
-      <c r="C98" t="s">
-        <v>212</v>
       </c>
       <c r="D98" t="s">
         <v>198</v>
       </c>
       <c r="E98" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F98" t="s">
         <v>199</v>
@@ -4618,7 +4672,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>132</v>
       </c>
@@ -4626,13 +4680,13 @@
         <v>133</v>
       </c>
       <c r="C99" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D99" t="s">
         <v>198</v>
       </c>
       <c r="E99" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F99" t="s">
         <v>134</v>
@@ -4641,7 +4695,7 @@
         <v>70</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>200</v>
+        <v>352</v>
       </c>
       <c r="I99" s="2" t="s">
         <v>123</v>
@@ -4652,58 +4706,58 @@
       <c r="L99" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M99" s="2" t="s">
+      <c r="N99" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
+        <v>321</v>
+      </c>
+      <c r="B100" t="s">
         <v>323</v>
       </c>
-      <c r="B100" t="s">
-        <v>325</v>
-      </c>
       <c r="C100" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D100" t="s">
         <v>198</v>
       </c>
       <c r="E100" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F100" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G100" t="s">
         <v>70</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="I100" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M100" s="2"/>
-    </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N100" s="2"/>
+    </row>
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B101" t="s">
         <v>61</v>
       </c>
       <c r="C101" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D101" t="s">
         <v>198</v>
       </c>
       <c r="E101" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F101" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G101" t="s">
         <v>70</v>
@@ -4720,34 +4774,34 @@
       <c r="L101" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M101" t="s">
+      <c r="N101" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B102" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C102" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D102" t="s">
         <v>198</v>
       </c>
       <c r="E102" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F102" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G102" t="s">
         <v>70</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="I102" s="2" t="s">
         <v>123</v>
@@ -4758,28 +4812,28 @@
       <c r="L102" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M102" t="s">
+      <c r="N102" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="B103" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C103" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D103" t="s">
         <v>198</v>
       </c>
       <c r="E103" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F103" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G103" t="s">
         <v>70</v>
@@ -4791,24 +4845,24 @@
         <v>123</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="B104" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D104" t="s">
         <v>198</v>
       </c>
       <c r="E104" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F104" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="G104" t="s">
         <v>70</v>

</xml_diff>

<commit_message>
RT fitting rework, update to minispectrum plots, isodist fitting with summed spectra
</commit_message>
<xml_diff>
--- a/pytheas_data/pytheas_global_parameters.xlsx
+++ b/pytheas_data/pytheas_global_parameters.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jrwill/prog/Pytheas_Folder/Pytheas_Qt_root/Pytheas_Qt/pytheas_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82121A6D-47F6-0B4F-B407-B2C324F1054C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBE93075-F768-1744-8F94-3D65284E1DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11200" yWindow="3840" windowWidth="35480" windowHeight="24200" xr2:uid="{5EC5A63B-1C8A-8A4B-9184-3058BFCD8B26}"/>
+    <workbookView xWindow="820" yWindow="760" windowWidth="28580" windowHeight="18360" xr2:uid="{5EC5A63B-1C8A-8A4B-9184-3058BFCD8B26}"/>
   </bookViews>
   <sheets>
     <sheet name="pytheas_button_parameters" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1134" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="424">
   <si>
     <t>missed_cleavages</t>
   </si>
@@ -1131,9 +1131,6 @@
     <t>Isodist Model Def File</t>
   </si>
   <si>
-    <t>isodist_label_model.txt</t>
-  </si>
-  <si>
     <t>Isodist Job</t>
   </si>
   <si>
@@ -1267,6 +1264,48 @@
   </si>
   <si>
     <t>Load RT index</t>
+  </si>
+  <si>
+    <t>isodist_fixed_N15_model.txt</t>
+  </si>
+  <si>
+    <t>Filter matches</t>
+  </si>
+  <si>
+    <t>filter_matches</t>
+  </si>
+  <si>
+    <t>Filter Matches</t>
+  </si>
+  <si>
+    <t>Match Filters file</t>
+  </si>
+  <si>
+    <t>match_filter_file</t>
+  </si>
+  <si>
+    <t>Match Filter File</t>
+  </si>
+  <si>
+    <t>read_filter_file</t>
+  </si>
+  <si>
+    <t>match_filter.xlsx</t>
+  </si>
+  <si>
+    <t>RT fit width</t>
+  </si>
+  <si>
+    <t>rt_fit_width</t>
+  </si>
+  <si>
+    <t>50,40,30,20</t>
+  </si>
+  <si>
+    <t>Fit Sum of Spectra</t>
+  </si>
+  <si>
+    <t>fit_sum_spectra</t>
   </si>
 </sst>
 </file>
@@ -1633,10 +1672,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA26392-E153-8845-A8FA-3CAC8BC5DFBF}">
-  <dimension ref="A1:N120"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:N124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="118" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScale="118" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="I96" sqref="I96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2489,7 +2529,7 @@
         <v>20</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -2875,10 +2915,10 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C39" t="s">
         <v>212</v>
@@ -2890,7 +2930,7 @@
         <v>348</v>
       </c>
       <c r="F39" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="G39" t="s">
         <v>56</v>
@@ -3894,42 +3934,42 @@
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>285</v>
+        <v>411</v>
       </c>
       <c r="B71" t="s">
-        <v>286</v>
+        <v>412</v>
       </c>
       <c r="C71" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D71" t="s">
         <v>162</v>
       </c>
       <c r="E71" t="s">
-        <v>287</v>
+        <v>160</v>
       </c>
       <c r="F71" t="s">
-        <v>288</v>
+        <v>413</v>
       </c>
       <c r="G71" t="s">
         <v>56</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="B72" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="C72" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="D72" t="s">
         <v>162</v>
@@ -3938,24 +3978,24 @@
         <v>287</v>
       </c>
       <c r="F72" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="G72" t="s">
-        <v>57</v>
-      </c>
-      <c r="H72" s="1">
-        <v>16</v>
-      </c>
-      <c r="I72" s="1">
-        <v>16</v>
+        <v>56</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B73" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C73" t="s">
         <v>214</v>
@@ -3967,27 +4007,27 @@
         <v>287</v>
       </c>
       <c r="F73" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="G73" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H73" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>16</v>
       </c>
       <c r="I73" s="1">
-        <v>7.4999999999999997E-2</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="B74" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="C74" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D74" t="s">
         <v>162</v>
@@ -3996,28 +4036,24 @@
         <v>287</v>
       </c>
       <c r="F74" t="s">
-        <v>297</v>
+        <v>284</v>
       </c>
       <c r="G74" t="s">
-        <v>58</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="L74" s="1"/>
-      <c r="M74" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="H74" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="I74" s="1">
+        <v>7.4999999999999997E-2</v>
+      </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="B75" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C75" t="s">
         <v>213</v>
@@ -4029,16 +4065,16 @@
         <v>287</v>
       </c>
       <c r="F75" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="G75" t="s">
         <v>58</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="I75" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
@@ -4047,10 +4083,10 @@
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>298</v>
+        <v>292</v>
       </c>
       <c r="B76" t="s">
-        <v>299</v>
+        <v>293</v>
       </c>
       <c r="C76" t="s">
         <v>213</v>
@@ -4062,16 +4098,16 @@
         <v>287</v>
       </c>
       <c r="F76" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="G76" t="s">
         <v>58</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
@@ -4080,13 +4116,13 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>339</v>
+        <v>298</v>
       </c>
       <c r="B77" t="s">
-        <v>339</v>
+        <v>299</v>
       </c>
       <c r="C77" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D77" t="s">
         <v>162</v>
@@ -4095,16 +4131,16 @@
         <v>287</v>
       </c>
       <c r="F77" t="s">
-        <v>340</v>
+        <v>300</v>
       </c>
       <c r="G77" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>68</v>
+        <v>295</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>20</v>
+        <v>295</v>
       </c>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
@@ -4113,10 +4149,10 @@
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>397</v>
+        <v>339</v>
       </c>
       <c r="B78" t="s">
-        <v>397</v>
+        <v>339</v>
       </c>
       <c r="C78" t="s">
         <v>212</v>
@@ -4128,7 +4164,7 @@
         <v>287</v>
       </c>
       <c r="F78" t="s">
-        <v>398</v>
+        <v>340</v>
       </c>
       <c r="G78" t="s">
         <v>56</v>
@@ -4146,42 +4182,46 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>235</v>
+        <v>396</v>
       </c>
       <c r="B79" t="s">
-        <v>242</v>
+        <v>396</v>
       </c>
       <c r="C79" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D79" t="s">
         <v>162</v>
       </c>
       <c r="E79" t="s">
-        <v>349</v>
+        <v>287</v>
       </c>
       <c r="F79" t="s">
-        <v>243</v>
+        <v>397</v>
       </c>
       <c r="G79" t="s">
         <v>56</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I79" s="2" t="s">
-        <v>71</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="I79" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J79" s="1"/>
+      <c r="K79" s="1"/>
+      <c r="L79" s="1"/>
+      <c r="M79" s="1"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="B80" t="s">
-        <v>189</v>
+        <v>242</v>
       </c>
       <c r="C80" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D80" t="s">
         <v>162</v>
@@ -4190,28 +4230,24 @@
         <v>349</v>
       </c>
       <c r="F80" t="s">
-        <v>190</v>
+        <v>243</v>
       </c>
       <c r="G80" t="s">
         <v>56</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I80" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
-      <c r="L80" s="1"/>
-      <c r="M80" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>301</v>
+        <v>189</v>
       </c>
       <c r="B81" t="s">
-        <v>302</v>
+        <v>189</v>
       </c>
       <c r="C81" t="s">
         <v>212</v>
@@ -4223,7 +4259,7 @@
         <v>349</v>
       </c>
       <c r="F81" t="s">
-        <v>312</v>
+        <v>190</v>
       </c>
       <c r="G81" t="s">
         <v>56</v>
@@ -4241,10 +4277,10 @@
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>244</v>
+        <v>301</v>
       </c>
       <c r="B82" t="s">
-        <v>244</v>
+        <v>302</v>
       </c>
       <c r="C82" t="s">
         <v>212</v>
@@ -4256,13 +4292,13 @@
         <v>349</v>
       </c>
       <c r="F82" t="s">
-        <v>245</v>
+        <v>312</v>
       </c>
       <c r="G82" t="s">
         <v>56</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I82" s="1" t="s">
         <v>20</v>
@@ -4274,10 +4310,10 @@
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="B83" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="C83" t="s">
         <v>212</v>
@@ -4289,7 +4325,7 @@
         <v>349</v>
       </c>
       <c r="F83" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="G83" t="s">
         <v>56</v>
@@ -4307,13 +4343,13 @@
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B84" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C84" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D84" t="s">
         <v>162</v>
@@ -4322,16 +4358,16 @@
         <v>349</v>
       </c>
       <c r="F84" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G84" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>241</v>
+        <v>66</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>241</v>
+        <v>20</v>
       </c>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
@@ -4340,31 +4376,31 @@
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>350</v>
+        <v>239</v>
       </c>
       <c r="B85" t="s">
-        <v>351</v>
+        <v>239</v>
       </c>
       <c r="C85" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="D85" t="s">
-        <v>350</v>
+        <v>162</v>
       </c>
       <c r="E85" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="F85" t="s">
-        <v>350</v>
+        <v>240</v>
       </c>
       <c r="G85" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>71</v>
+        <v>241</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>71</v>
+        <v>241</v>
       </c>
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
@@ -4373,13 +4409,13 @@
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>374</v>
+        <v>350</v>
       </c>
       <c r="B86" t="s">
-        <v>375</v>
+        <v>351</v>
       </c>
       <c r="C86" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="D86" t="s">
         <v>350</v>
@@ -4388,16 +4424,16 @@
         <v>352</v>
       </c>
       <c r="F86" t="s">
-        <v>376</v>
+        <v>350</v>
       </c>
       <c r="G86" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>378</v>
+        <v>71</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>377</v>
+        <v>71</v>
       </c>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
@@ -4406,13 +4442,13 @@
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>399</v>
+        <v>373</v>
       </c>
       <c r="B87" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="C87" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D87" t="s">
         <v>350</v>
@@ -4421,16 +4457,16 @@
         <v>352</v>
       </c>
       <c r="F87" t="s">
-        <v>410</v>
+        <v>375</v>
       </c>
       <c r="G87" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>68</v>
+        <v>377</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>20</v>
+        <v>376</v>
       </c>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
@@ -4439,10 +4475,10 @@
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>380</v>
+        <v>398</v>
       </c>
       <c r="B88" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C88" t="s">
         <v>212</v>
@@ -4454,7 +4490,7 @@
         <v>352</v>
       </c>
       <c r="F88" t="s">
-        <v>380</v>
+        <v>409</v>
       </c>
       <c r="G88" t="s">
         <v>56</v>
@@ -4472,10 +4508,10 @@
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>406</v>
+        <v>379</v>
       </c>
       <c r="B89" t="s">
-        <v>408</v>
+        <v>380</v>
       </c>
       <c r="C89" t="s">
         <v>212</v>
@@ -4487,7 +4523,7 @@
         <v>352</v>
       </c>
       <c r="F89" t="s">
-        <v>406</v>
+        <v>379</v>
       </c>
       <c r="G89" t="s">
         <v>56</v>
@@ -4505,10 +4541,10 @@
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
+        <v>405</v>
+      </c>
+      <c r="B90" t="s">
         <v>407</v>
-      </c>
-      <c r="B90" t="s">
-        <v>409</v>
       </c>
       <c r="C90" t="s">
         <v>212</v>
@@ -4520,7 +4556,7 @@
         <v>352</v>
       </c>
       <c r="F90" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="G90" t="s">
         <v>56</v>
@@ -4534,16 +4570,14 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
-      <c r="M90" s="1" t="s">
-        <v>346</v>
-      </c>
+      <c r="M90" s="1"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>383</v>
+        <v>406</v>
       </c>
       <c r="B91" t="s">
-        <v>384</v>
+        <v>408</v>
       </c>
       <c r="C91" t="s">
         <v>212</v>
@@ -4555,28 +4589,30 @@
         <v>352</v>
       </c>
       <c r="F91" t="s">
-        <v>383</v>
+        <v>406</v>
       </c>
       <c r="G91" t="s">
         <v>56</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>382</v>
+        <v>68</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>390</v>
+        <v>20</v>
       </c>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
-      <c r="M91" s="1"/>
+      <c r="M91" s="1" t="s">
+        <v>346</v>
+      </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="B92" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C92" t="s">
         <v>212</v>
@@ -4588,13 +4624,13 @@
         <v>352</v>
       </c>
       <c r="F92" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="G92" t="s">
         <v>56</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>389</v>
@@ -4606,13 +4642,13 @@
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="B93" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="C93" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D93" t="s">
         <v>350</v>
@@ -4621,16 +4657,16 @@
         <v>352</v>
       </c>
       <c r="F93" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G93" t="s">
-        <v>59</v>
-      </c>
-      <c r="H93" s="1">
-        <v>0.98</v>
-      </c>
-      <c r="I93" s="1">
-        <v>0.98</v>
+        <v>56</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>388</v>
       </c>
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
@@ -4639,31 +4675,31 @@
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>248</v>
+        <v>390</v>
       </c>
       <c r="B94" t="s">
-        <v>249</v>
+        <v>391</v>
       </c>
       <c r="C94" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D94" t="s">
-        <v>246</v>
+        <v>350</v>
       </c>
       <c r="E94" t="s">
-        <v>247</v>
+        <v>352</v>
       </c>
       <c r="F94" t="s">
-        <v>248</v>
+        <v>392</v>
       </c>
       <c r="G94" t="s">
-        <v>58</v>
-      </c>
-      <c r="H94" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="I94" s="1" t="s">
-        <v>329</v>
+        <v>59</v>
+      </c>
+      <c r="H94" s="1">
+        <v>0.98</v>
+      </c>
+      <c r="I94" s="1">
+        <v>0.98</v>
       </c>
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
@@ -4672,31 +4708,31 @@
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>255</v>
+        <v>419</v>
       </c>
       <c r="B95" t="s">
-        <v>256</v>
+        <v>420</v>
       </c>
       <c r="C95" t="s">
         <v>212</v>
       </c>
       <c r="D95" t="s">
-        <v>246</v>
+        <v>350</v>
       </c>
       <c r="E95" t="s">
-        <v>247</v>
+        <v>352</v>
       </c>
       <c r="F95" t="s">
-        <v>257</v>
+        <v>419</v>
       </c>
       <c r="G95" t="s">
         <v>57</v>
       </c>
       <c r="H95" s="1">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>258</v>
+        <v>421</v>
       </c>
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
@@ -4705,31 +4741,31 @@
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>259</v>
+        <v>422</v>
       </c>
       <c r="B96" t="s">
-        <v>260</v>
+        <v>423</v>
       </c>
       <c r="C96" t="s">
         <v>212</v>
       </c>
       <c r="D96" t="s">
-        <v>246</v>
+        <v>350</v>
       </c>
       <c r="E96" t="s">
-        <v>247</v>
+        <v>352</v>
       </c>
       <c r="F96" t="s">
-        <v>259</v>
+        <v>422</v>
       </c>
       <c r="G96" t="s">
-        <v>57</v>
-      </c>
-      <c r="H96" s="1">
-        <v>1</v>
+        <v>56</v>
+      </c>
+      <c r="H96" s="1" t="s">
+        <v>66</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>65</v>
+        <v>20</v>
       </c>
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
@@ -4738,13 +4774,13 @@
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>331</v>
+        <v>248</v>
       </c>
       <c r="B97" t="s">
-        <v>332</v>
+        <v>249</v>
       </c>
       <c r="C97" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D97" t="s">
         <v>246</v>
@@ -4753,16 +4789,16 @@
         <v>247</v>
       </c>
       <c r="F97" t="s">
-        <v>331</v>
+        <v>248</v>
       </c>
       <c r="G97" t="s">
-        <v>57</v>
-      </c>
-      <c r="H97" s="1">
-        <v>1000</v>
-      </c>
-      <c r="I97" s="1">
-        <v>1000</v>
+        <v>58</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>329</v>
       </c>
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
@@ -4771,10 +4807,10 @@
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>338</v>
+        <v>255</v>
       </c>
       <c r="B98" t="s">
-        <v>336</v>
+        <v>256</v>
       </c>
       <c r="C98" t="s">
         <v>212</v>
@@ -4786,16 +4822,16 @@
         <v>247</v>
       </c>
       <c r="F98" t="s">
-        <v>337</v>
+        <v>257</v>
       </c>
       <c r="G98" t="s">
-        <v>56</v>
-      </c>
-      <c r="H98" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
+      </c>
+      <c r="H98" s="1">
+        <v>16</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>20</v>
+        <v>258</v>
       </c>
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
@@ -4804,13 +4840,13 @@
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>333</v>
+        <v>259</v>
       </c>
       <c r="B99" t="s">
-        <v>334</v>
+        <v>260</v>
       </c>
       <c r="C99" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D99" t="s">
         <v>246</v>
@@ -4819,176 +4855,152 @@
         <v>247</v>
       </c>
       <c r="F99" t="s">
-        <v>333</v>
+        <v>259</v>
       </c>
       <c r="G99" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H99" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="I99" s="2" t="s">
-        <v>335</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J99" s="1"/>
+      <c r="K99" s="1"/>
+      <c r="L99" s="1"/>
+      <c r="M99" s="1"/>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>402</v>
+        <v>331</v>
       </c>
       <c r="B100" t="s">
-        <v>403</v>
+        <v>332</v>
       </c>
       <c r="C100" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="D100" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="E100" t="s">
-        <v>400</v>
+        <v>247</v>
       </c>
       <c r="F100" t="s">
-        <v>139</v>
+        <v>331</v>
       </c>
       <c r="G100" t="s">
-        <v>56</v>
-      </c>
-      <c r="H100" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I100" s="2" t="s">
-        <v>71</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H100" s="1">
+        <v>1000</v>
+      </c>
+      <c r="I100" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J100" s="1"/>
+      <c r="K100" s="1"/>
+      <c r="L100" s="1"/>
+      <c r="M100" s="1"/>
     </row>
     <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>125</v>
+        <v>338</v>
       </c>
       <c r="B101" t="s">
-        <v>127</v>
+        <v>336</v>
       </c>
       <c r="C101" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D101" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="E101" t="s">
-        <v>400</v>
+        <v>247</v>
       </c>
       <c r="F101" t="s">
-        <v>125</v>
+        <v>337</v>
       </c>
       <c r="G101" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="I101" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="J101" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="K101" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="L101" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="N101" t="s">
-        <v>101</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>97</v>
+        <v>333</v>
       </c>
       <c r="B102" t="s">
-        <v>98</v>
+        <v>334</v>
       </c>
       <c r="C102" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D102" t="s">
-        <v>196</v>
+        <v>246</v>
       </c>
       <c r="E102" t="s">
-        <v>400</v>
+        <v>247</v>
       </c>
       <c r="F102" t="s">
-        <v>99</v>
+        <v>333</v>
       </c>
       <c r="G102" t="s">
-        <v>70</v>
-      </c>
-      <c r="H102" s="1" t="s">
-        <v>100</v>
+        <v>59</v>
+      </c>
+      <c r="H102" s="1">
+        <v>0.2</v>
       </c>
       <c r="I102" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="J102" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="K102" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="L102" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="N102" t="s">
-        <v>101</v>
+        <v>335</v>
       </c>
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>108</v>
+        <v>401</v>
       </c>
       <c r="B103" t="s">
-        <v>114</v>
+        <v>402</v>
       </c>
       <c r="C103" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D103" t="s">
         <v>196</v>
       </c>
       <c r="E103" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F103" t="s">
-        <v>108</v>
+        <v>139</v>
       </c>
       <c r="G103" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>109</v>
+        <v>71</v>
       </c>
       <c r="I103" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="J103" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="K103" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="L103" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="N103" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="B104" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="C104" t="s">
         <v>211</v>
@@ -4997,22 +5009,22 @@
         <v>196</v>
       </c>
       <c r="E104" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F104" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="G104" t="s">
         <v>70</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="I104" s="2" t="s">
         <v>216</v>
       </c>
       <c r="J104" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="K104" s="2" t="s">
         <v>120</v>
@@ -5026,10 +5038,10 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>164</v>
+        <v>97</v>
       </c>
       <c r="B105" t="s">
-        <v>165</v>
+        <v>98</v>
       </c>
       <c r="C105" t="s">
         <v>211</v>
@@ -5038,22 +5050,22 @@
         <v>196</v>
       </c>
       <c r="E105" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F105" t="s">
-        <v>166</v>
+        <v>99</v>
       </c>
       <c r="G105" t="s">
         <v>70</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>167</v>
+        <v>100</v>
       </c>
       <c r="I105" s="2" t="s">
         <v>216</v>
       </c>
       <c r="J105" s="2" t="s">
-        <v>163</v>
+        <v>150</v>
       </c>
       <c r="K105" s="2" t="s">
         <v>120</v>
@@ -5067,10 +5079,10 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>220</v>
+        <v>108</v>
       </c>
       <c r="B106" t="s">
-        <v>221</v>
+        <v>114</v>
       </c>
       <c r="C106" t="s">
         <v>211</v>
@@ -5079,22 +5091,22 @@
         <v>196</v>
       </c>
       <c r="E106" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="F106" t="s">
-        <v>222</v>
+        <v>108</v>
       </c>
       <c r="G106" t="s">
         <v>70</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>223</v>
+        <v>109</v>
       </c>
       <c r="I106" s="2" t="s">
         <v>216</v>
       </c>
       <c r="J106" s="2" t="s">
-        <v>224</v>
+        <v>148</v>
       </c>
       <c r="K106" s="2" t="s">
         <v>120</v>
@@ -5102,45 +5114,57 @@
       <c r="L106" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="N106" s="2" t="s">
+      <c r="N106" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>404</v>
+        <v>110</v>
       </c>
       <c r="B107" t="s">
-        <v>405</v>
+        <v>111</v>
       </c>
       <c r="C107" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D107" t="s">
         <v>196</v>
       </c>
       <c r="E107" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F107" t="s">
-        <v>142</v>
+        <v>112</v>
       </c>
       <c r="G107" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>71</v>
+        <v>113</v>
       </c>
       <c r="I107" s="2" t="s">
-        <v>71</v>
+        <v>216</v>
+      </c>
+      <c r="J107" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K107" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L107" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="N107" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>250</v>
+        <v>164</v>
       </c>
       <c r="B108" t="s">
-        <v>251</v>
+        <v>165</v>
       </c>
       <c r="C108" t="s">
         <v>211</v>
@@ -5149,22 +5173,22 @@
         <v>196</v>
       </c>
       <c r="E108" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F108" t="s">
-        <v>252</v>
+        <v>166</v>
       </c>
       <c r="G108" t="s">
         <v>70</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>253</v>
+        <v>167</v>
       </c>
       <c r="I108" s="2" t="s">
         <v>216</v>
       </c>
       <c r="J108" s="2" t="s">
-        <v>254</v>
+        <v>163</v>
       </c>
       <c r="K108" s="2" t="s">
         <v>120</v>
@@ -5172,16 +5196,16 @@
       <c r="L108" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="N108" s="2" t="s">
-        <v>326</v>
+      <c r="N108" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>357</v>
+        <v>220</v>
       </c>
       <c r="B109" t="s">
-        <v>358</v>
+        <v>221</v>
       </c>
       <c r="C109" t="s">
         <v>211</v>
@@ -5190,130 +5214,133 @@
         <v>196</v>
       </c>
       <c r="E109" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F109" t="s">
-        <v>359</v>
+        <v>222</v>
       </c>
       <c r="G109" t="s">
         <v>70</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>360</v>
+        <v>223</v>
       </c>
       <c r="I109" s="2" t="s">
-        <v>361</v>
+        <v>216</v>
       </c>
       <c r="J109" s="2" t="s">
-        <v>373</v>
+        <v>224</v>
       </c>
       <c r="K109" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>122</v>
+        <v>199</v>
       </c>
       <c r="N109" s="2" t="s">
-        <v>326</v>
+        <v>101</v>
       </c>
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>362</v>
+        <v>403</v>
       </c>
       <c r="B110" t="s">
-        <v>363</v>
+        <v>404</v>
       </c>
       <c r="C110" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D110" t="s">
         <v>196</v>
       </c>
       <c r="E110" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="F110" t="s">
-        <v>364</v>
+        <v>142</v>
       </c>
       <c r="G110" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>365</v>
+        <v>71</v>
       </c>
       <c r="I110" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="J110" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="K110" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="L110" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="N110" s="2" t="s">
-        <v>326</v>
+        <v>71</v>
       </c>
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>207</v>
+        <v>250</v>
       </c>
       <c r="B111" t="s">
-        <v>208</v>
+        <v>251</v>
       </c>
       <c r="C111" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D111" t="s">
         <v>196</v>
       </c>
       <c r="E111" t="s">
-        <v>231</v>
+        <v>400</v>
       </c>
       <c r="F111" t="s">
-        <v>197</v>
+        <v>252</v>
       </c>
       <c r="G111" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>71</v>
+        <v>253</v>
       </c>
       <c r="I111" s="2" t="s">
-        <v>71</v>
+        <v>216</v>
+      </c>
+      <c r="J111" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="K111" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="L111" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="N111" s="2" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>131</v>
+        <v>414</v>
       </c>
       <c r="B112" t="s">
-        <v>132</v>
+        <v>415</v>
       </c>
       <c r="C112" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D112" t="s">
         <v>196</v>
       </c>
       <c r="E112" t="s">
-        <v>231</v>
+        <v>400</v>
       </c>
       <c r="F112" t="s">
-        <v>133</v>
+        <v>416</v>
       </c>
       <c r="G112" t="s">
         <v>70</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>345</v>
+        <v>418</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>122</v>
+        <v>216</v>
+      </c>
+      <c r="J112" s="2" t="s">
+        <v>417</v>
       </c>
       <c r="K112" s="2" t="s">
         <v>118</v>
@@ -5322,66 +5349,80 @@
         <v>122</v>
       </c>
       <c r="N112" s="2" t="s">
-        <v>103</v>
+        <v>326</v>
       </c>
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>318</v>
+        <v>357</v>
       </c>
       <c r="B113" t="s">
-        <v>320</v>
+        <v>358</v>
       </c>
       <c r="C113" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D113" t="s">
         <v>196</v>
       </c>
       <c r="E113" t="s">
-        <v>231</v>
+        <v>400</v>
       </c>
       <c r="F113" t="s">
-        <v>318</v>
+        <v>359</v>
       </c>
       <c r="G113" t="s">
         <v>70</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>319</v>
+        <v>360</v>
       </c>
       <c r="I113" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="J113" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="K113" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L113" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="N113" s="2"/>
+      <c r="N113" s="2" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>321</v>
+        <v>362</v>
       </c>
       <c r="B114" t="s">
-        <v>61</v>
+        <v>363</v>
       </c>
       <c r="C114" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D114" t="s">
         <v>196</v>
       </c>
       <c r="E114" t="s">
-        <v>231</v>
+        <v>400</v>
       </c>
       <c r="F114" t="s">
-        <v>321</v>
+        <v>364</v>
       </c>
       <c r="G114" t="s">
         <v>70</v>
       </c>
       <c r="H114" s="1" t="s">
-        <v>188</v>
+        <v>410</v>
       </c>
       <c r="I114" s="2" t="s">
-        <v>122</v>
+        <v>361</v>
+      </c>
+      <c r="J114" s="2" t="s">
+        <v>372</v>
       </c>
       <c r="K114" s="2" t="s">
         <v>118</v>
@@ -5389,19 +5430,19 @@
       <c r="L114" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="N114" t="s">
-        <v>102</v>
+      <c r="N114" s="2" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>232</v>
+        <v>207</v>
       </c>
       <c r="B115" t="s">
-        <v>267</v>
+        <v>208</v>
       </c>
       <c r="C115" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D115" t="s">
         <v>196</v>
@@ -5410,33 +5451,24 @@
         <v>231</v>
       </c>
       <c r="F115" t="s">
-        <v>234</v>
+        <v>197</v>
       </c>
       <c r="G115" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="H115" s="1" t="s">
-        <v>233</v>
+        <v>71</v>
       </c>
       <c r="I115" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="K115" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="L115" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="N115" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>370</v>
+        <v>131</v>
       </c>
       <c r="B116" t="s">
-        <v>371</v>
+        <v>132</v>
       </c>
       <c r="C116" t="s">
         <v>215</v>
@@ -5448,13 +5480,13 @@
         <v>231</v>
       </c>
       <c r="F116" t="s">
-        <v>370</v>
+        <v>133</v>
       </c>
       <c r="G116" t="s">
         <v>70</v>
       </c>
       <c r="H116" s="1" t="s">
-        <v>372</v>
+        <v>345</v>
       </c>
       <c r="I116" s="2" t="s">
         <v>122</v>
@@ -5465,16 +5497,16 @@
       <c r="L116" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="N116" t="s">
-        <v>102</v>
+      <c r="N116" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="B117" t="s">
-        <v>314</v>
+        <v>320</v>
       </c>
       <c r="C117" t="s">
         <v>215</v>
@@ -5486,33 +5518,25 @@
         <v>231</v>
       </c>
       <c r="F117" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
       <c r="G117" t="s">
         <v>70</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>71</v>
+        <v>319</v>
       </c>
       <c r="I117" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="K117" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="L117" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="N117" t="s">
-        <v>102</v>
-      </c>
+      <c r="N117" s="2"/>
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="B118" t="s">
-        <v>316</v>
+        <v>61</v>
       </c>
       <c r="C118" t="s">
         <v>215</v>
@@ -5524,13 +5548,13 @@
         <v>231</v>
       </c>
       <c r="F118" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="G118" t="s">
         <v>70</v>
       </c>
       <c r="H118" s="1" t="s">
-        <v>71</v>
+        <v>188</v>
       </c>
       <c r="I118" s="2" t="s">
         <v>122</v>
@@ -5547,10 +5571,10 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>366</v>
+        <v>232</v>
       </c>
       <c r="B119" t="s">
-        <v>367</v>
+        <v>267</v>
       </c>
       <c r="C119" t="s">
         <v>215</v>
@@ -5562,13 +5586,13 @@
         <v>231</v>
       </c>
       <c r="F119" t="s">
-        <v>366</v>
+        <v>234</v>
       </c>
       <c r="G119" t="s">
         <v>70</v>
       </c>
       <c r="H119" s="1" t="s">
-        <v>71</v>
+        <v>233</v>
       </c>
       <c r="I119" s="2" t="s">
         <v>122</v>
@@ -5585,10 +5609,10 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="B120" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="C120" t="s">
         <v>215</v>
@@ -5600,13 +5624,13 @@
         <v>231</v>
       </c>
       <c r="F120" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G120" t="s">
         <v>70</v>
       </c>
       <c r="H120" s="1" t="s">
-        <v>71</v>
+        <v>371</v>
       </c>
       <c r="I120" s="2" t="s">
         <v>122</v>
@@ -5618,6 +5642,158 @@
         <v>122</v>
       </c>
       <c r="N120" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>313</v>
+      </c>
+      <c r="B121" t="s">
+        <v>314</v>
+      </c>
+      <c r="C121" t="s">
+        <v>215</v>
+      </c>
+      <c r="D121" t="s">
+        <v>196</v>
+      </c>
+      <c r="E121" t="s">
+        <v>231</v>
+      </c>
+      <c r="F121" t="s">
+        <v>313</v>
+      </c>
+      <c r="G121" t="s">
+        <v>70</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I121" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="K121" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L121" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N121" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>315</v>
+      </c>
+      <c r="B122" t="s">
+        <v>316</v>
+      </c>
+      <c r="C122" t="s">
+        <v>215</v>
+      </c>
+      <c r="D122" t="s">
+        <v>196</v>
+      </c>
+      <c r="E122" t="s">
+        <v>231</v>
+      </c>
+      <c r="F122" t="s">
+        <v>317</v>
+      </c>
+      <c r="G122" t="s">
+        <v>70</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I122" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="K122" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L122" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N122" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>365</v>
+      </c>
+      <c r="B123" t="s">
+        <v>366</v>
+      </c>
+      <c r="C123" t="s">
+        <v>215</v>
+      </c>
+      <c r="D123" t="s">
+        <v>196</v>
+      </c>
+      <c r="E123" t="s">
+        <v>231</v>
+      </c>
+      <c r="F123" t="s">
+        <v>365</v>
+      </c>
+      <c r="G123" t="s">
+        <v>70</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I123" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="K123" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L123" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N123" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A124" t="s">
+        <v>367</v>
+      </c>
+      <c r="B124" t="s">
+        <v>368</v>
+      </c>
+      <c r="C124" t="s">
+        <v>215</v>
+      </c>
+      <c r="D124" t="s">
+        <v>196</v>
+      </c>
+      <c r="E124" t="s">
+        <v>231</v>
+      </c>
+      <c r="F124" t="s">
+        <v>367</v>
+      </c>
+      <c r="G124" t="s">
+        <v>70</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="I124" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="K124" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="L124" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="N124" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>